<commit_message>
data: fix d5x device eventbook incorrect
</commit_message>
<xml_diff>
--- a/foxlink_dispatch/test_data/D5X Device 事件簿[修正].xlsx
+++ b/foxlink_dispatch/test_data/D5X Device 事件簿[修正].xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20383"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ethan\SimsLab\正崴 Foxlink\程式碼_Code\演算法 Algorithm 建構[2]\#原始資料\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\School Projects\Foxlink\API_Backend\foxlink_dispatch\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A861D2A-8526-4741-881E-6C3F3177CD7A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C650C6-072F-46C5-9DEE-A058DBCAEC1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2145" windowWidth="28800" windowHeight="12435" tabRatio="500" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2250" yWindow="4080" windowWidth="23475" windowHeight="15345" tabRatio="500" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Device_1" sheetId="3" r:id="rId1"/>
@@ -134,7 +134,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="288">
   <si>
     <t>优先顺序</t>
   </si>
@@ -998,10 +998,6 @@
   </si>
   <si>
     <t>MESSAGE</t>
-  </si>
-  <si>
-    <t>MESSAGE2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2506,8 +2502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -2522,7 +2518,7 @@
         <v>286</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>0</v>
@@ -3333,7 +3329,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="108" zoomScalePageLayoutView="108" workbookViewId="0">
+    <sheetView zoomScale="108" zoomScaleNormal="108" zoomScalePageLayoutView="108" workbookViewId="0">
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>

</xml_diff>